<commit_message>
Text changes for bulk receipt recovery (#765)
</commit_message>
<xml_diff>
--- a/src/EA.Iws.Api/Documents/BulkUploadReceiptRecoveryTemplate.xlsx
+++ b/src/EA.Iws.Api/Documents/BulkUploadReceiptRecoveryTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="http://teamshare1.ea.gov/directorates/EandB/IWSRFH/Shared Documents/IWS Online/3. BETA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source Code\IWS\src\EA.Iws.Api\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -52,9 +52,6 @@
     <t>This is a numerical field and must contain whole numbers. The number must be the shipment number of the prenotification</t>
   </si>
   <si>
-    <t>This column should be in a numerical format; no more than 4 decimal places</t>
-  </si>
-  <si>
     <t>This is a textual field. The unit of measurement must be written as, for example, Tonnes or m3</t>
   </si>
   <si>
@@ -75,11 +72,14 @@
   <si>
     <t>Received</t>
   </si>
+  <si>
+    <t>This column must be in a numerical format; no more than 4 decimal places for measurements in Tonnes or 1 decimal place for measurements in Kilograms</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -443,16 +443,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -6440,7 +6440,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:F17"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6448,13 +6448,13 @@
     <col min="1" max="1" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -6462,21 +6462,21 @@
         <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6487,16 +6487,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -12585,15 +12585,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007759CA8CE08AB9419CDC954FF1613187" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="471c13ecf6b8d239f1a9ed47c0d50475">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36541348-b42e-4df6-937f-59ca2d1235b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="199054d83c20ad432576f091e08ce527" ns2:_="">
     <xsd:import namespace="36541348-b42e-4df6-937f-59ca2d1235b1"/>
@@ -12719,6 +12710,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0899E7A-4D4B-43DA-B6AE-C0F9946C6508}">
   <ds:schemaRefs>
@@ -12736,14 +12736,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2C1C823-8EC4-49EB-865C-E57F6F836890}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CCD4673-6493-47A9-92C0-83CC8866F933}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12759,4 +12751,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2C1C823-8EC4-49EB-865C-E57F6F836890}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update text on guidance sheet for receipt recovery.
</commit_message>
<xml_diff>
--- a/src/EA.Iws.Api/Documents/BulkUploadReceiptRecoveryTemplate.xlsx
+++ b/src/EA.Iws.Api/Documents/BulkUploadReceiptRecoveryTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source Code\IWS\src\EA.Iws.Api\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EA\prsd-iws\src\EA.Iws.Api\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -46,9 +46,6 @@
     <t>Please note that if you use the template file to arrange your data into the correct format, the sheet containing the data for upload must be positioned as the first sheet within the whole workbook. Alternatively, you could create a local version of this template with only one sheet and popoulate your data as appropriate.</t>
   </si>
   <si>
-    <t>This is a textual field and will contain the notification number with no blank spaces</t>
-  </si>
-  <si>
     <t>This is a numerical field and must contain whole numbers. The number must be the shipment number of the prenotification</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>This column must be in a numerical format; no more than 4 decimal places for measurements in Tonnes or 1 decimal place for measurements in Kilograms</t>
+  </si>
+  <si>
+    <t>This is a textual field and will contain the notification number</t>
   </si>
 </sst>
 </file>
@@ -138,8 +138,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -443,16 +471,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -6440,7 +6468,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6454,29 +6482,29 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6487,16 +6515,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -12577,11 +12605,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-17T08:24:03+00:00</Date>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12711,26 +12740,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-17T08:24:03+00:00</Date>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0899E7A-4D4B-43DA-B6AE-C0F9946C6508}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2C1C823-8EC4-49EB-865C-E57F6F836890}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12754,9 +12774,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2C1C823-8EC4-49EB-865C-E57F6F836890}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0899E7A-4D4B-43DA-B6AE-C0F9946C6508}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Bulk receipt recovery bug fixes (#824)
* Pad missing last column for receipt recovery for CSV since this is optional and could be easily missed out.

* Update validation message for the checking recovery/disposed date is in future and after received date.

* Update validation rules to return message if shipment does not already exist.

* Update text on guidance sheet for receipt recovery.
</commit_message>
<xml_diff>
--- a/src/EA.Iws.Api/Documents/BulkUploadReceiptRecoveryTemplate.xlsx
+++ b/src/EA.Iws.Api/Documents/BulkUploadReceiptRecoveryTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source Code\IWS\src\EA.Iws.Api\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EA\prsd-iws\src\EA.Iws.Api\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -46,9 +46,6 @@
     <t>Please note that if you use the template file to arrange your data into the correct format, the sheet containing the data for upload must be positioned as the first sheet within the whole workbook. Alternatively, you could create a local version of this template with only one sheet and popoulate your data as appropriate.</t>
   </si>
   <si>
-    <t>This is a textual field and will contain the notification number with no blank spaces</t>
-  </si>
-  <si>
     <t>This is a numerical field and must contain whole numbers. The number must be the shipment number of the prenotification</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>This column must be in a numerical format; no more than 4 decimal places for measurements in Tonnes or 1 decimal place for measurements in Kilograms</t>
+  </si>
+  <si>
+    <t>This is a textual field and will contain the notification number</t>
   </si>
 </sst>
 </file>
@@ -138,8 +138,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -443,16 +471,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -6440,7 +6468,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6454,29 +6482,29 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6487,16 +6515,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -12577,11 +12605,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-17T08:24:03+00:00</Date>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12711,26 +12740,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-17T08:24:03+00:00</Date>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0899E7A-4D4B-43DA-B6AE-C0F9946C6508}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2C1C823-8EC4-49EB-865C-E57F6F836890}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12754,9 +12774,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2C1C823-8EC4-49EB-865C-E57F6F836890}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0899E7A-4D4B-43DA-B6AE-C0F9946C6508}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>